<commit_message>
multi-agent 는 collision X -> ERROR
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_1/Curriculum No ob train 5000_1_Test_multi_agent/Curriculum No ob train 5000_1_Test_multi_agent_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_1/Curriculum No ob train 5000_1_Test_multi_agent/Curriculum No ob train 5000_1_Test_multi_agent_Test_Result.xlsx
@@ -448,10 +448,10 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.925</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
this model test velocity change 1.57,3.14,6.28
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_1/Curriculum No ob train 5000_1_Test_multi_agent/Curriculum No ob train 5000_1_Test_multi_agent_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum No ob train 5000_1/Curriculum No ob train 5000_1_Test_multi_agent/Curriculum No ob train 5000_1_Test_multi_agent_Test_Result.xlsx
@@ -448,10 +448,10 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>

</xml_diff>